<commit_message>
Correccion de bat para finReport, creacion de DAG importa_mantenedores
</commit_message>
<xml_diff>
--- a/contenedores/airflow/mantenedores/interfaz_manager.xlsx
+++ b/contenedores/airflow/mantenedores/interfaz_manager.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\airflow\finReport\mantenedores\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/78ec6eafe1d282b6/Felipe/Projects/CMF/finReport/contenedores/airflow/mantenedores/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED31AA9-16CE-4DDF-BD4B-6EE5C242270D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{EED31AA9-16CE-4DDF-BD4B-6EE5C242270D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4203797C-02B1-4313-A90C-7B22D86A46E1}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="interfaz_manager" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -206,16 +206,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -507,14 +504,14 @@
   <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection sqref="A1:D50"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="1"/>
     <col min="2" max="3" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.21875" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
@@ -528,7 +525,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>45</v>
       </c>
     </row>
@@ -640,7 +637,7 @@
       <c r="C9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>36</v>
       </c>
     </row>
@@ -654,7 +651,7 @@
       <c r="C10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>35</v>
       </c>
     </row>
@@ -668,7 +665,7 @@
       <c r="C11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>36</v>
       </c>
     </row>
@@ -682,7 +679,7 @@
       <c r="C12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>35</v>
       </c>
     </row>
@@ -696,7 +693,7 @@
       <c r="C13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="3" t="s">
         <v>35</v>
       </c>
     </row>
@@ -710,7 +707,7 @@
       <c r="C14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="3" t="s">
         <v>35</v>
       </c>
     </row>
@@ -724,7 +721,7 @@
       <c r="C15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="3" t="s">
         <v>35</v>
       </c>
     </row>
@@ -738,7 +735,7 @@
       <c r="C16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="3" t="s">
         <v>35</v>
       </c>
     </row>
@@ -752,7 +749,7 @@
       <c r="C17" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="3" t="s">
         <v>35</v>
       </c>
     </row>
@@ -766,7 +763,7 @@
       <c r="C18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="3" t="s">
         <v>35</v>
       </c>
     </row>
@@ -780,7 +777,7 @@
       <c r="C19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="3" t="s">
         <v>35</v>
       </c>
     </row>
@@ -794,7 +791,7 @@
       <c r="C20" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="3" t="s">
         <v>34</v>
       </c>
     </row>
@@ -808,7 +805,7 @@
       <c r="C21" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="3" t="s">
         <v>34</v>
       </c>
     </row>
@@ -822,7 +819,7 @@
       <c r="C22" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="3" t="s">
         <v>34</v>
       </c>
     </row>
@@ -836,7 +833,7 @@
       <c r="C23" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="3" t="s">
         <v>34</v>
       </c>
     </row>
@@ -850,7 +847,7 @@
       <c r="C24" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="3" t="s">
         <v>36</v>
       </c>
     </row>
@@ -864,7 +861,7 @@
       <c r="C25" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="3" t="s">
         <v>36</v>
       </c>
     </row>
@@ -878,7 +875,7 @@
       <c r="C26" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="3" t="s">
         <v>34</v>
       </c>
     </row>
@@ -892,7 +889,7 @@
       <c r="C27" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="3" t="s">
         <v>34</v>
       </c>
     </row>
@@ -906,7 +903,7 @@
       <c r="C28" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="3" t="s">
         <v>35</v>
       </c>
     </row>
@@ -917,10 +914,10 @@
       <c r="B29" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="3" t="s">
         <v>36</v>
       </c>
     </row>
@@ -931,7 +928,7 @@
       <c r="B30" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D30" s="3" t="s">
@@ -945,10 +942,10 @@
       <c r="B31" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="3" t="s">
         <v>36</v>
       </c>
     </row>
@@ -959,7 +956,7 @@
       <c r="B32" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D32" s="3" t="s">
@@ -973,7 +970,7 @@
       <c r="B33" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="4" t="s">
         <v>39</v>
       </c>
       <c r="D33" s="3" t="s">
@@ -987,7 +984,7 @@
       <c r="B34" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="4" t="s">
         <v>40</v>
       </c>
       <c r="D34" s="3" t="s">
@@ -1001,7 +998,7 @@
       <c r="B35" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D35" s="3" t="s">
@@ -1015,7 +1012,7 @@
       <c r="B36" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="4" t="s">
         <v>42</v>
       </c>
       <c r="D36" s="3" t="s">
@@ -1029,7 +1026,7 @@
       <c r="B37" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C37" s="4" t="s">
         <v>43</v>
       </c>
       <c r="D37" s="3" t="s">
@@ -1043,7 +1040,7 @@
       <c r="B38" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C38" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D38" s="3" t="s">
@@ -1060,7 +1057,7 @@
       <c r="C39" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D39" s="3" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1074,7 +1071,7 @@
       <c r="C40" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D40" s="6" t="s">
+      <c r="D40" s="5" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1088,7 +1085,7 @@
       <c r="C41" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D41" s="6" t="s">
+      <c r="D41" s="5" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1102,7 +1099,7 @@
       <c r="C42" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="D42" s="3" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1116,7 +1113,7 @@
       <c r="C43" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="D43" s="3" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1186,7 +1183,7 @@
       <c r="C48" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D48" s="4" t="s">
+      <c r="D48" s="3" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se modifica tabla interfaz_manager por interfaz e interfaz_rel, se incorpora en log_eventos de donde proviene el proceso si de DAG o procedimiento almacenado
</commit_message>
<xml_diff>
--- a/contenedores/airflow/mantenedores/interfaz_manager.xlsx
+++ b/contenedores/airflow/mantenedores/interfaz_manager.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/78ec6eafe1d282b6/Felipe/Projects/CMF/finReport/contenedores/airflow/mantenedores/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{EED31AA9-16CE-4DDF-BD4B-6EE5C242270D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4203797C-02B1-4313-A90C-7B22D86A46E1}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="13_ncr:1_{EED31AA9-16CE-4DDF-BD4B-6EE5C242270D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{136AAE05-991B-425B-A33C-26D77B384744}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="interfaz_manager" sheetId="1" r:id="rId1"/>
+    <sheet name="interfaz" sheetId="3" r:id="rId1"/>
+    <sheet name="interfaz_rel" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="54">
   <si>
     <t>interfaz</t>
   </si>
@@ -166,6 +167,27 @@
   </si>
   <si>
     <t>cuadro_rectificaciones</t>
+  </si>
+  <si>
+    <t>cod</t>
+  </si>
+  <si>
+    <t>msi</t>
+  </si>
+  <si>
+    <t>A01</t>
+  </si>
+  <si>
+    <t>B01</t>
+  </si>
+  <si>
+    <t>C01</t>
+  </si>
+  <si>
+    <t>D01</t>
+  </si>
+  <si>
+    <t>REDEC</t>
   </si>
 </sst>
 </file>
@@ -236,6 +258,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -500,18 +526,95 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D50"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8A910D5-DE0F-4E9E-8E14-825D182FE3F8}">
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="3" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="3" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
@@ -520,7 +623,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -534,7 +637,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
@@ -548,7 +651,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
@@ -562,7 +665,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>13</v>
@@ -576,7 +679,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>5</v>
@@ -590,7 +693,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>14</v>
@@ -604,7 +707,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>15</v>
@@ -618,7 +721,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>16</v>
@@ -632,7 +735,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>17</v>
@@ -646,7 +749,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>18</v>
@@ -660,7 +763,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>19</v>
@@ -674,7 +777,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>20</v>
@@ -688,7 +791,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>21</v>
@@ -702,7 +805,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>22</v>
@@ -716,7 +819,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>23</v>
@@ -730,7 +833,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>24</v>
@@ -744,7 +847,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>25</v>
@@ -758,7 +861,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>26</v>
@@ -772,7 +875,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>27</v>
@@ -786,7 +889,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>28</v>
@@ -800,7 +903,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>29</v>
@@ -814,7 +917,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>30</v>
@@ -828,7 +931,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>31</v>
@@ -842,7 +945,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>4</v>
@@ -856,7 +959,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>9</v>
@@ -870,7 +973,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>10</v>
@@ -884,7 +987,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>11</v>
@@ -898,7 +1001,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>32</v>
@@ -912,7 +1015,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>3</v>
@@ -926,7 +1029,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>5</v>
@@ -940,7 +1043,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>38</v>
@@ -954,7 +1057,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>25</v>
@@ -968,7 +1071,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>39</v>
@@ -982,7 +1085,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>40</v>
@@ -996,7 +1099,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>41</v>
@@ -1010,7 +1113,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>42</v>
@@ -1024,7 +1127,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>43</v>
@@ -1038,7 +1141,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>27</v>
@@ -1052,7 +1155,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>3</v>
@@ -1066,7 +1169,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>28</v>
@@ -1080,7 +1183,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>8</v>
@@ -1094,7 +1197,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>3</v>
@@ -1108,7 +1211,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>4</v>
@@ -1122,7 +1225,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>5</v>
@@ -1136,7 +1239,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>6</v>
@@ -1150,7 +1253,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>7</v>
@@ -1164,7 +1267,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>8</v>
@@ -1178,7 +1281,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>9</v>
@@ -1192,7 +1295,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>10</v>
@@ -1206,7 +1309,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Avance en DAG para importar interfaces import_interfaz.py
</commit_message>
<xml_diff>
--- a/contenedores/airflow/mantenedores/interfaz_manager.xlsx
+++ b/contenedores/airflow/mantenedores/interfaz_manager.xlsx
@@ -530,7 +530,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -606,7 +606,7 @@
   <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Avance en logica de determinacion de la mora sin aceleracion
</commit_message>
<xml_diff>
--- a/contenedores/airflow/mantenedores/interfaz_manager.xlsx
+++ b/contenedores/airflow/mantenedores/interfaz_manager.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/78ec6eafe1d282b6/Felipe/Projects/CMF/finReport/contenedores/airflow/mantenedores/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{EED31AA9-16CE-4DDF-BD4B-6EE5C242270D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A9E80AA-8932-4B59-8280-8D3BDF56F545}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="13_ncr:1_{EED31AA9-16CE-4DDF-BD4B-6EE5C242270D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AFD6725F-FB44-42FB-ABAB-4680407621CE}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -132,9 +132,6 @@
     <t>deuda_renegociada</t>
   </si>
   <si>
-    <t>operación_desfasada</t>
-  </si>
-  <si>
     <t>valor_contable</t>
   </si>
   <si>
@@ -199,6 +196,9 @@
   </si>
   <si>
     <t>REDEC</t>
+  </si>
+  <si>
+    <t>operacion_desfasada</t>
   </si>
 </sst>
 </file>
@@ -554,57 +554,57 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -617,7 +617,7 @@
   <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29:C38"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -634,13 +634,13 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
@@ -648,13 +648,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
@@ -662,13 +662,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
@@ -676,13 +676,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
@@ -690,13 +690,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
@@ -704,13 +704,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
@@ -718,13 +718,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
@@ -732,13 +732,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
@@ -746,13 +746,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
@@ -760,13 +760,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
@@ -774,13 +774,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
@@ -788,13 +788,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
@@ -802,13 +802,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
@@ -816,13 +816,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
@@ -830,13 +830,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
@@ -844,13 +844,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
@@ -858,13 +858,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
@@ -872,13 +872,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
@@ -886,13 +886,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
@@ -900,13 +900,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>28</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
@@ -914,13 +914,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
@@ -928,13 +928,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
@@ -942,13 +942,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
@@ -956,13 +956,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
@@ -970,13 +970,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
@@ -984,13 +984,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
@@ -998,13 +998,13 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
@@ -1012,13 +1012,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
@@ -1026,13 +1026,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
@@ -1040,13 +1040,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
@@ -1054,13 +1054,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">
@@ -1068,13 +1068,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
@@ -1082,13 +1082,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
@@ -1096,13 +1096,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
@@ -1110,13 +1110,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
@@ -1124,13 +1124,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.15">
@@ -1138,13 +1138,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.15">
@@ -1152,13 +1152,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.15">
@@ -1166,13 +1166,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.15">
@@ -1180,13 +1180,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>28</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
@@ -1194,13 +1194,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.15">
@@ -1208,13 +1208,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.15">
@@ -1222,13 +1222,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
@@ -1236,13 +1236,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
@@ -1250,13 +1250,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
@@ -1264,13 +1264,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
@@ -1278,13 +1278,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
@@ -1292,13 +1292,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
@@ -1306,13 +1306,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.15">
@@ -1320,13 +1320,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambios en algunas tablas y procedimientos por incorporacion de interfaz de cartera_garantias
</commit_message>
<xml_diff>
--- a/contenedores/airflow/mantenedores/interfaz_manager.xlsx
+++ b/contenedores/airflow/mantenedores/interfaz_manager.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/78ec6eafe1d282b6/Felipe/Projects/CMF/finReport/contenedores/airflow/mantenedores/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="71" documentId="13_ncr:1_{EED31AA9-16CE-4DDF-BD4B-6EE5C242270D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B00ACCFB-EB84-4297-AD96-778E1FA3823B}"/>
+  <xr:revisionPtr revIDLastSave="72" documentId="13_ncr:1_{EED31AA9-16CE-4DDF-BD4B-6EE5C242270D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC3D8AAA-6FF4-47A1-99E4-794AE41C123D}"/>
   <bookViews>
-    <workbookView xWindow="13590" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="interfaz" sheetId="3" r:id="rId1"/>
@@ -564,8 +564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8A910D5-DE0F-4E9E-8E14-825D182FE3F8}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -651,7 +651,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47:C60"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
@@ -748,7 +750,6 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
-        <f>A6+1</f>
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -763,7 +764,6 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="1">
-        <f t="shared" ref="A8:A60" si="0">A7+1</f>
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -778,7 +778,6 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="1">
-        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -793,7 +792,6 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="1">
-        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -808,7 +806,6 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="1">
-        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -823,7 +820,6 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" s="1">
-        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -838,7 +834,6 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="1">
-        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -853,7 +848,6 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="1">
-        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -868,7 +862,6 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="1">
-        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -883,7 +876,6 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" s="1">
-        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -898,7 +890,6 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="1">
-        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -913,7 +904,6 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="1">
-        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -928,7 +918,6 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" s="1">
-        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -943,7 +932,6 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="1">
-        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -958,7 +946,6 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" s="1">
-        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -973,7 +960,6 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" s="1">
-        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -988,7 +974,6 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" s="1">
-        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1003,7 +988,6 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" s="1">
-        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -1018,7 +1002,6 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25" s="1">
-        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -1033,7 +1016,6 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26" s="1">
-        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -1048,7 +1030,6 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27" s="1">
-        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -1063,7 +1044,6 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" s="1">
-        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -1078,7 +1058,6 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29" s="1">
-        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -1093,7 +1072,6 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A30" s="1">
-        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -1108,7 +1086,6 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31" s="1">
-        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -1123,7 +1100,6 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A32" s="1">
-        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -1138,7 +1114,6 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A33" s="1">
-        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -1153,7 +1128,6 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A34" s="1">
-        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -1168,7 +1142,6 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A35" s="1">
-        <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -1183,7 +1156,6 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A36" s="1">
-        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -1198,7 +1170,6 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A37" s="1">
-        <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -1213,7 +1184,6 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A38" s="1">
-        <f t="shared" si="0"/>
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -1228,7 +1198,6 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A39" s="1">
-        <f t="shared" si="0"/>
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
@@ -1243,7 +1212,6 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A40" s="1">
-        <f t="shared" si="0"/>
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -1258,7 +1226,6 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A41" s="1">
-        <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -1273,7 +1240,6 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A42" s="1">
-        <f t="shared" si="0"/>
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
@@ -1288,7 +1254,6 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A43" s="1">
-        <f t="shared" si="0"/>
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
@@ -1303,7 +1268,6 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A44" s="1">
-        <f t="shared" si="0"/>
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -1318,7 +1282,6 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A45" s="1">
-        <f t="shared" si="0"/>
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -1333,7 +1296,6 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A46" s="1">
-        <f t="shared" si="0"/>
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -1348,7 +1310,6 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A47" s="1">
-        <f t="shared" si="0"/>
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
@@ -1363,7 +1324,6 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A48" s="1">
-        <f t="shared" si="0"/>
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
@@ -1378,7 +1338,6 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A49" s="1">
-        <f t="shared" si="0"/>
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
@@ -1393,7 +1352,6 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A50" s="1">
-        <f t="shared" si="0"/>
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -1408,7 +1366,6 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A51" s="1">
-        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
@@ -1423,7 +1380,6 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A52" s="1">
-        <f t="shared" si="0"/>
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -1438,7 +1394,6 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A53" s="1">
-        <f t="shared" si="0"/>
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
@@ -1453,7 +1408,6 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A54" s="1">
-        <f t="shared" si="0"/>
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
@@ -1468,7 +1422,6 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A55" s="1">
-        <f t="shared" si="0"/>
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
@@ -1483,7 +1436,6 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A56" s="1">
-        <f t="shared" si="0"/>
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -1498,7 +1450,6 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A57" s="1">
-        <f t="shared" si="0"/>
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
@@ -1513,7 +1464,6 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A58" s="1">
-        <f t="shared" si="0"/>
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
@@ -1528,7 +1478,6 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A59" s="1">
-        <f t="shared" si="0"/>
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
@@ -1543,7 +1492,6 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A60" s="1">
-        <f t="shared" si="0"/>
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">

</xml_diff>